<commit_message>
vault backup: 2023-08-02 17:17:39
</commit_message>
<xml_diff>
--- a/Mechanics structures and materials/THING_SHEET.xlsx
+++ b/Mechanics structures and materials/THING_SHEET.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni stuff\Uni notes\Mechanics structures and materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni stuff\Uni-notes\Mechanics structures and materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5873179B-AD2F-49F8-8BCE-55FEBA76857E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE61D6C-0645-4F2F-801A-A55B33E14DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{B4832339-B459-4DE3-BBF5-0C74B6145684}"/>
+    <workbookView minimized="1" xWindow="3540" yWindow="3525" windowWidth="12690" windowHeight="9360" activeTab="2" xr2:uid="{B4832339-B459-4DE3-BBF5-0C74B6145684}"/>
   </bookViews>
   <sheets>
     <sheet name="Beam cross section (2)" sheetId="3" r:id="rId1"/>
     <sheet name="Beam cross section" sheetId="1" r:id="rId2"/>
-    <sheet name="Energy cons" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
-    <sheet name="Composites" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
+    <sheet name="Energy cons" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
+    <sheet name="Composites" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="139">
   <si>
     <t>Calculated values</t>
   </si>
@@ -444,6 +445,42 @@
   <si>
     <t>U</t>
   </si>
+  <si>
+    <t>SiC Fibre</t>
+  </si>
+  <si>
+    <t>Al2 O3 fibre</t>
+  </si>
+  <si>
+    <t>Carbon Fibre</t>
+  </si>
+  <si>
+    <t>Tungsten</t>
+  </si>
+  <si>
+    <t>Youngs mod (Gpa)</t>
+  </si>
+  <si>
+    <t>Yield strength (Mpa)</t>
+  </si>
+  <si>
+    <t>Density (g/cm^3)</t>
+  </si>
+  <si>
+    <t>Fibre volume fraction</t>
+  </si>
+  <si>
+    <t>Composite YM (Gpa)</t>
+  </si>
+  <si>
+    <t>Composite Yield (Mpa)</t>
+  </si>
+  <si>
+    <t>Specific Comp YM</t>
+  </si>
+  <si>
+    <t>Specific Comp Yield</t>
+  </si>
 </sst>
 </file>
 
@@ -513,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -586,11 +623,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -628,6 +683,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -649,7 +705,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1278,7 +1338,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.1</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,10 +1350,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>12.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1340,7 +1400,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.1</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,10 +1412,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>11.1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.1</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1376,10 +1436,10 @@
               <c:strCache>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>12.7</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.7</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1413,10 +1473,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>12.7</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.7</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,10 +1488,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>12.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,10 +1535,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>12.7</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.7</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1490,10 +1550,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>11.1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.1</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8278,25 +8338,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="15.75" customHeight="1">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="22"/>
+      <c r="V2" s="23"/>
       <c r="W2" s="11"/>
       <c r="X2" s="2" t="s">
         <v>17</v>
@@ -9308,10 +9368,10 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R18" s="23" t="s">
+      <c r="R18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="S18" s="23"/>
+      <c r="S18" s="24"/>
       <c r="U18" s="2">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -9437,10 +9497,10 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="N20" s="23" t="s">
+      <c r="N20" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="O20" s="23"/>
+      <c r="O20" s="24"/>
       <c r="R20" s="2" t="s">
         <v>42</v>
       </c>
@@ -10454,8 +10514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645780B6-C6D9-4438-A108-DEE3BF26AAE1}">
   <dimension ref="B1:AE39"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10485,19 +10545,19 @@
       </c>
     </row>
     <row r="2" spans="2:31" ht="15.75" customHeight="1">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="T2" s="2" t="s">
@@ -10506,10 +10566,10 @@
       <c r="U2" s="2">
         <v>2700</v>
       </c>
-      <c r="Y2" s="21" t="s">
+      <c r="Y2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="22"/>
+      <c r="Z2" s="23"/>
       <c r="AA2" s="11"/>
       <c r="AB2" s="2" t="s">
         <v>17</v>
@@ -10557,14 +10617,14 @@
       </c>
       <c r="O3" s="6">
         <f>SUM(H4:H35)</f>
-        <v>38.079999999999984</v>
+        <v>700</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="Q3" s="3">
         <f>O3/1000^2</f>
-        <v>3.8079999999999981E-5</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
@@ -10593,49 +10653,48 @@
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>12.7</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
-        <v>12.7</v>
+        <v>100</v>
       </c>
       <c r="E4" s="7">
-        <f>12.7-1.6</f>
-        <v>11.1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1">
         <f>ABS(C4-E4)</f>
-        <v>1.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1">
         <f>ABS(D4-B4)</f>
-        <v>12.7</v>
+        <v>100</v>
       </c>
       <c r="H4" s="1">
         <f>F4*G4</f>
-        <v>20.319999999999993</v>
+        <v>500</v>
       </c>
       <c r="I4" s="1">
         <f>(B4+D4)/2</f>
-        <v>6.35</v>
+        <v>50</v>
       </c>
       <c r="J4" s="1">
         <f>(C4+E4)/2</f>
-        <v>11.899999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="K4" s="1">
         <f>H4*I4</f>
-        <v>129.03199999999995</v>
+        <v>25000</v>
       </c>
       <c r="L4" s="1">
         <f>H4*J4</f>
-        <v>241.80799999999988</v>
+        <v>1250</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>47</v>
       </c>
       <c r="O4" s="6">
         <f>SUM(K4:K35)/O3</f>
-        <v>8.9384453781512612</v>
+        <v>55.714285714285715</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>15</v>
@@ -10649,76 +10708,76 @@
       </c>
       <c r="Y4" s="2">
         <f>(F4^3*G4/12) + H4*ABS(J4-$O$5)^2</f>
-        <v>182.55770674622758</v>
+        <v>113541.66666666667</v>
       </c>
       <c r="Z4" s="2">
         <f>(G4^3*F4/12) + H4*(I4-$O$4)^2</f>
-        <v>409.26273867900102</v>
+        <v>432993.1972789116</v>
       </c>
       <c r="AA4" s="2">
         <f>H4*(I4-$O$4)*(J4-$O$5)</f>
-        <v>-155.76951062071879</v>
+        <v>42857.14285714287</v>
       </c>
       <c r="AB4" s="2">
         <f t="shared" ref="AB4:AB35" si="0">MAX(F4:G4)</f>
-        <v>12.7</v>
+        <v>100</v>
       </c>
       <c r="AC4" s="2">
         <f t="shared" ref="AC4:AC35" si="1">MIN(F4:G4)</f>
-        <v>1.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="AD4" s="2">
         <f>AB4^3*AC4</f>
-        <v>3277.4127999999992</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="5" spans="2:31">
       <c r="B5" s="8">
-        <v>11.1</v>
+        <v>69</v>
       </c>
       <c r="C5" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5" s="8">
-        <v>12.7</v>
+        <v>71</v>
       </c>
       <c r="E5" s="8">
-        <v>11.1</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1">
         <f>ABS(C5-E5)</f>
-        <v>11.1</v>
+        <v>100</v>
       </c>
       <c r="G5" s="1">
         <f>ABS(D5-B5)</f>
-        <v>1.5999999999999996</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1">
         <f>F5*G5</f>
-        <v>17.759999999999994</v>
+        <v>200</v>
       </c>
       <c r="I5" s="1">
         <f>(B5+D5)/2</f>
-        <v>11.899999999999999</v>
+        <v>70</v>
       </c>
       <c r="J5" s="1">
         <f>(C5+E5)/2</f>
-        <v>5.55</v>
+        <v>55</v>
       </c>
       <c r="K5" s="1">
         <f>H5*I5</f>
-        <v>211.34399999999991</v>
+        <v>14000</v>
       </c>
       <c r="L5" s="1">
         <f>H5*J5</f>
-        <v>98.567999999999969</v>
+        <v>11000</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="O5" s="6">
         <f>SUM(L4:L35)/O3</f>
-        <v>8.9384453781512612</v>
+        <v>17.5</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>15</v>
@@ -10732,27 +10791,27 @@
       </c>
       <c r="Y5" s="2">
         <f>(F5^3*G5/12) + H5*ABS(J5-$O$5)^2</f>
-        <v>386.26334255349195</v>
+        <v>447916.66666666663</v>
       </c>
       <c r="Z5" s="2">
         <f>(G5^3*F5/12) + H5*(I5-$O$4)^2</f>
-        <v>159.5583106207186</v>
+        <v>40882.993197278905</v>
       </c>
       <c r="AA5" s="2">
         <f t="shared" ref="AA5:AA35" si="2">H5*(I5-$O$4)*(J5-$O$5)</f>
-        <v>-178.22277341289444</v>
+        <v>107142.85714285713</v>
       </c>
       <c r="AB5" s="2">
         <f t="shared" si="0"/>
-        <v>11.1</v>
+        <v>100</v>
       </c>
       <c r="AC5" s="2">
         <f t="shared" si="1"/>
-        <v>1.5999999999999996</v>
+        <v>2</v>
       </c>
       <c r="AD5" s="2">
         <f t="shared" ref="AD5:AD35" si="3">AB5^3*AC5</f>
-        <v>2188.2095999999992</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="6" spans="2:31">
@@ -10851,7 +10910,7 @@
       </c>
       <c r="U7" s="2">
         <f>Q3*U2*U3*(U4+U5)^2/2 + U1*(U4+U5)</f>
-        <v>4.0005512943315198</v>
+        <v>5.2797411458000001</v>
       </c>
       <c r="Y7" s="2">
         <f t="shared" si="11"/>
@@ -10916,7 +10975,7 @@
       </c>
       <c r="U8" s="2">
         <f>U1+(U5+U4)*Q3*U3*U2-U7</f>
-        <v>6.66474344038848</v>
+        <v>12.082882654200002</v>
       </c>
       <c r="Y8" s="2">
         <f t="shared" si="11"/>
@@ -10984,14 +11043,14 @@
       </c>
       <c r="O9" s="2">
         <f>SUM(AA4:AA35)</f>
-        <v>-333.99228403361326</v>
+        <v>150000</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="Q9" s="2">
         <f>O9*1000^-4</f>
-        <v>-3.3399228403361326E-10</v>
+        <v>1.4999999999999999E-7</v>
       </c>
       <c r="R9" s="12" t="s">
         <v>64</v>
@@ -11059,14 +11118,14 @@
       </c>
       <c r="O10" s="6">
         <f>SUM(Y4:Y35)</f>
-        <v>568.82104929971956</v>
+        <v>561458.33333333326</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="Q10" s="2">
         <f t="shared" ref="Q10:Q12" si="13">O10*1000^-4</f>
-        <v>5.6882104929971957E-10</v>
+        <v>5.6145833333333329E-7</v>
       </c>
       <c r="R10" s="12" t="s">
         <v>64</v>
@@ -11076,7 +11135,7 @@
       </c>
       <c r="U10" s="2">
         <f>-((U8*U4^2)/6 + (U2*Q3*U3/24) *U4^3)</f>
-        <v>-5.4572887413705928E-3</v>
+        <v>-1.0132667863430004E-2</v>
       </c>
       <c r="W10" s="2" t="s">
         <v>84</v>
@@ -11148,14 +11207,14 @@
       </c>
       <c r="O11" s="6">
         <f>SUM(Z4:Z35)</f>
-        <v>568.82104929971956</v>
+        <v>473876.19047619053</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="Q11" s="2">
         <f t="shared" si="13"/>
-        <v>5.6882104929971957E-10</v>
+        <v>4.7387619047619054E-7</v>
       </c>
       <c r="R11" s="12" t="s">
         <v>64</v>
@@ -11165,14 +11224,14 @@
       </c>
       <c r="U11" s="2">
         <f>U8/6</f>
-        <v>1.1107905733980801</v>
+        <v>2.0138137757000005</v>
       </c>
       <c r="W11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11" s="2" t="e">
         <f>(U11*X10^3 + U12*X10^4 + (X10-U4)^3*U13+(U10*X10))*U14</f>
-        <v>3.1534161264779276E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y11" s="2">
         <f t="shared" si="11"/>
@@ -11240,14 +11299,14 @@
       </c>
       <c r="O12" s="2">
         <f>SUM(AD4:AD35)</f>
-        <v>5465.6223999999984</v>
+        <v>7000000</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="2">
         <f t="shared" si="13"/>
-        <v>5.4656223999999979E-9</v>
+        <v>6.9999999999999999E-6</v>
       </c>
       <c r="R12" s="12" t="s">
         <v>64</v>
@@ -11257,11 +11316,11 @@
       </c>
       <c r="U12" s="2">
         <f>Q3*U2*U3/24</f>
-        <v>4.202603999999998E-2</v>
-      </c>
-      <c r="X12" s="2">
+        <v>0.77253749999999999</v>
+      </c>
+      <c r="X12" s="2" t="e">
         <f>X11*1000</f>
-        <v>3.1534161264779277</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y12" s="2">
         <f t="shared" si="11"/>
@@ -11326,11 +11385,11 @@
       </c>
       <c r="U13" s="2">
         <f>U7/6</f>
-        <v>0.66675854905525334</v>
-      </c>
-      <c r="X13" s="2">
+        <v>0.87995685763333331</v>
+      </c>
+      <c r="X13" s="2" t="e">
         <f>(U11*X10^3 + U12*X10^4 +(U10*X10))*U14</f>
-        <v>2.3648473934940223E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y13" s="2">
         <f t="shared" si="11"/>
@@ -11393,13 +11452,13 @@
       <c r="T14" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U14" s="2" t="e">
         <f>Q11/(O23*(Q10*Q11-Q9^2))</f>
-        <v>3.8941007021137432E-2</v>
-      </c>
-      <c r="X14" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X14" s="2" t="e">
         <f>X13*1000</f>
-        <v>2.3648473934940224</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y14" s="2">
         <f t="shared" si="11"/>
@@ -11642,10 +11701,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T18" s="23" t="s">
+      <c r="T18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="U18" s="23"/>
+      <c r="U18" s="24"/>
       <c r="Y18" s="2">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -11771,10 +11830,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N20" s="23" t="s">
+      <c r="N20" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="O20" s="23"/>
+      <c r="O20" s="24"/>
       <c r="T20" s="2" t="s">
         <v>42</v>
       </c>
@@ -11846,7 +11905,7 @@
         <v>50</v>
       </c>
       <c r="O21" s="14">
-        <v>-3.21</v>
+        <v>0</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>54</v>
@@ -11998,8 +12057,7 @@
         <v>23</v>
       </c>
       <c r="O23" s="14">
-        <f>68.9*10^9</f>
-        <v>68900000000</v>
+        <v>0</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>60</v>
@@ -12009,7 +12067,7 @@
       </c>
       <c r="U23" s="2">
         <f>1000^4*((O21*O11-O22*O9))/(O11*O10-O9*O9)</f>
-        <v>-8612543581.8579445</v>
+        <v>0</v>
       </c>
       <c r="V23" s="12" t="s">
         <v>59</v>
@@ -12078,7 +12136,7 @@
         <v>65</v>
       </c>
       <c r="O24" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="P24" s="12" t="s">
         <v>53</v>
@@ -12088,7 +12146,7 @@
       </c>
       <c r="U24" s="2">
         <f>1000^4*((O22*O10-O21*O9))/(O11*O10-O9*O9)</f>
-        <v>-5056991308.2244129</v>
+        <v>0</v>
       </c>
       <c r="V24" s="2" t="s">
         <v>59</v>
@@ -12156,7 +12214,7 @@
       </c>
       <c r="U25" s="2">
         <f>((O21*O11-O22*O9)*U22+(O22*O10-O21*O9)*U21)/(O11*O10-O9*O9)</f>
-        <v>-6.5526257000442012E-2</v>
+        <v>0</v>
       </c>
       <c r="Y25" s="2">
         <f t="shared" si="11"/>
@@ -12218,7 +12276,7 @@
       </c>
       <c r="U26" s="2">
         <f>((U23*U22/1000)+(U24*U21)/1000)/1000^2</f>
-        <v>-65.526257000441987</v>
+        <v>0</v>
       </c>
       <c r="V26" s="12" t="s">
         <v>61</v>
@@ -12402,9 +12460,9 @@
       <c r="N29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O29" s="2">
+      <c r="O29" s="2" t="e">
         <f>ATAN( -(O22*O10-O21*O9)/(O21*O11-O22*O9) )</f>
-        <v>-0.53092915895002402</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>40</v>
@@ -12473,9 +12531,9 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O30" s="2">
+      <c r="O30" s="2" t="e">
         <f>O29*180/PI()</f>
-        <v>-30.420000028266813</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>38</v>
@@ -12483,20 +12541,20 @@
       <c r="T30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="U30" s="2">
+      <c r="U30" s="2" t="e">
         <f>Q11/(O23*(Q11*Q10-Q9*Q9))</f>
-        <v>3.8941007021137432E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="V30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="W30" s="2">
+      <c r="W30" s="2" t="e">
         <f>-U30*10.28*0.312/2</f>
-        <v>-6.2448914139657669E-2</v>
-      </c>
-      <c r="X30" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X30" s="2" t="e">
         <f>W30/1000^2</f>
-        <v>-6.2448914139657665E-8</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y30" s="2">
         <f t="shared" si="11"/>
@@ -12559,16 +12617,16 @@
       <c r="N31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="O31" s="2">
+      <c r="O31" s="2" t="e">
         <f>(O23*(Q11*Q10-Q9^2))/(O21*Q11-O22*Q9)</f>
-        <v>-7.9999595177823775</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q31" s="2">
+      <c r="Q31" s="2" t="e">
         <f>O31*1000</f>
-        <v>-7999.9595177823776</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R31" s="2" t="s">
         <v>15</v>
@@ -12576,13 +12634,13 @@
       <c r="V31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="W31" s="2">
+      <c r="W31" s="2" t="e">
         <f>U30*10.28/6</f>
-        <v>6.6718925362882125E-2</v>
-      </c>
-      <c r="X31" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X31" s="2" t="e">
         <f>W31/1000^3</f>
-        <v>6.6718925362882128E-11</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y31" s="2">
         <f t="shared" si="11"/>
@@ -12645,16 +12703,16 @@
       <c r="N32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O32" s="2">
+      <c r="O32" s="2" t="e">
         <f>(O23*(Q11*Q10-Q9^2))/(O22*Q10-O21*Q9)</f>
-        <v>-13.624702080848911</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P32" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q32" s="2">
+      <c r="Q32" s="2" t="e">
         <f>O32*1000</f>
-        <v>-13624.702080848911</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R32" s="2" t="s">
         <v>15</v>
@@ -12720,16 +12778,16 @@
       <c r="N33" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="O33" s="2">
+      <c r="O33" s="2" t="e">
         <f>(-1/O31)*0.5</f>
-        <v>6.250031626892559E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P33" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Q33" s="2">
+      <c r="Q33" s="2" t="e">
         <f>O33*1000</f>
-        <v>62.500316268925587</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R33" s="2" t="s">
         <v>71</v>
@@ -12737,20 +12795,20 @@
       <c r="T33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="U33" s="2">
+      <c r="U33" s="2" t="e">
         <f>-Q9/(O23*(Q11*Q10-Q9*Q9))</f>
-        <v>2.2864828742836529E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="V33" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="W33" s="2">
+      <c r="W33" s="2" t="e">
         <f>-U33*10.28*0.312/2</f>
-        <v>-3.6667868558312083E-2</v>
-      </c>
-      <c r="X33" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X33" s="2" t="e">
         <f t="shared" ref="X33" si="14">W33/1000^2</f>
-        <v>-3.6667868558312085E-8</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y33" s="2">
         <f t="shared" si="11"/>
@@ -12813,16 +12871,16 @@
       <c r="N34" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="O34" s="2">
+      <c r="O34" s="2" t="e">
         <f>(-1/O32)*0.5</f>
-        <v>3.6698050132252628E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P34" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Q34" s="2">
+      <c r="Q34" s="2" t="e">
         <f>O34*1000</f>
-        <v>36.698050132252625</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R34" s="12" t="s">
         <v>71</v>
@@ -12830,13 +12888,13 @@
       <c r="V34" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="W34" s="2">
+      <c r="W34" s="2" t="e">
         <f>U33*10.28/6</f>
-        <v>3.917507324605992E-2</v>
-      </c>
-      <c r="X34" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X34" s="2" t="e">
         <f>W34/1000^3</f>
-        <v>3.9175073246059917E-11</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y34" s="2">
         <f t="shared" si="11"/>
@@ -12899,9 +12957,9 @@
       <c r="N35" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="O35" s="2">
+      <c r="O35" s="2" t="e">
         <f>O33*O24^2</f>
-        <v>5.6250284642033032E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P35" s="12" t="s">
         <v>53</v>
@@ -12935,9 +12993,9 @@
       <c r="N36" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="O36" s="2">
+      <c r="O36" s="2" t="e">
         <f>O34*O24^2</f>
-        <v>3.3028245119027366E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P36" s="12" t="s">
         <v>53</v>
@@ -12965,26 +13023,26 @@
       <c r="V38" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="W38" s="2">
+      <c r="W38" s="2" t="e">
         <f>X30*W37^2+X31*W37^3</f>
-        <v>-3.9357947760256624E-3</v>
-      </c>
-      <c r="Y38" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y38" s="2" t="e">
         <f>W30*Y37^2+W31*Y37^3</f>
-        <v>-3.9357947760256633E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="2:30">
       <c r="V39" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="W39" s="2">
+      <c r="W39" s="2" t="e">
         <f>X33*W37^2+X34*W37^3</f>
-        <v>-2.3109642098348821E-3</v>
-      </c>
-      <c r="Y39" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y39" s="2" t="e">
         <f>W33*Y37^2+W34*Y37^3</f>
-        <v>-2.3109642098348817E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -13003,11 +13061,636 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D845C7-FAC7-45A7-9B9A-402BF8379545}">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1">
+        <v>0.3</v>
+      </c>
+      <c r="C1">
+        <v>0.3</v>
+      </c>
+      <c r="D1">
+        <v>0.3</v>
+      </c>
+      <c r="E1">
+        <v>0.3</v>
+      </c>
+      <c r="F1">
+        <v>0.4</v>
+      </c>
+      <c r="G1">
+        <v>0.4</v>
+      </c>
+      <c r="H1">
+        <v>0.4</v>
+      </c>
+      <c r="I1">
+        <v>0.4</v>
+      </c>
+      <c r="J1">
+        <v>0.5</v>
+      </c>
+      <c r="K1">
+        <v>0.5</v>
+      </c>
+      <c r="L1">
+        <v>0.5</v>
+      </c>
+      <c r="M1">
+        <v>0.5</v>
+      </c>
+      <c r="N1">
+        <v>0.32</v>
+      </c>
+      <c r="O1">
+        <v>0.32</v>
+      </c>
+      <c r="P1">
+        <v>0.32</v>
+      </c>
+      <c r="Q1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="B6" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="29">
+        <v>0.4</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="29">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="B7" s="28"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="29"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="B8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="28">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.95</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="29">
+        <v>19.3</v>
+      </c>
+      <c r="F9" s="28">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3.95</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="29">
+        <v>19.3</v>
+      </c>
+      <c r="J9" s="28">
+        <v>3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>3.95</v>
+      </c>
+      <c r="L9" s="2">
+        <v>2</v>
+      </c>
+      <c r="M9" s="29">
+        <v>19.3</v>
+      </c>
+      <c r="N9" s="28">
+        <v>3</v>
+      </c>
+      <c r="O9" s="2">
+        <v>3.95</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="29">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="28">
+        <v>400</v>
+      </c>
+      <c r="C10" s="2">
+        <v>379</v>
+      </c>
+      <c r="D10" s="2">
+        <v>500</v>
+      </c>
+      <c r="E10" s="29">
+        <v>407</v>
+      </c>
+      <c r="F10" s="28">
+        <v>400</v>
+      </c>
+      <c r="G10" s="2">
+        <v>379</v>
+      </c>
+      <c r="H10" s="2">
+        <v>500</v>
+      </c>
+      <c r="I10" s="29">
+        <v>407</v>
+      </c>
+      <c r="J10" s="28">
+        <v>400</v>
+      </c>
+      <c r="K10" s="2">
+        <v>379</v>
+      </c>
+      <c r="L10" s="2">
+        <v>500</v>
+      </c>
+      <c r="M10" s="29">
+        <v>407</v>
+      </c>
+      <c r="N10" s="28">
+        <v>400</v>
+      </c>
+      <c r="O10" s="2">
+        <v>379</v>
+      </c>
+      <c r="P10" s="2">
+        <v>500</v>
+      </c>
+      <c r="Q10" s="29">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="28">
+        <v>3900</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1380</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E11" s="29">
+        <v>2890</v>
+      </c>
+      <c r="F11" s="28">
+        <v>3900</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1380</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="29">
+        <v>2890</v>
+      </c>
+      <c r="J11" s="28">
+        <v>3900</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1380</v>
+      </c>
+      <c r="L11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M11" s="29">
+        <v>2890</v>
+      </c>
+      <c r="N11" s="28">
+        <v>3900</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1380</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="Q11" s="29">
+        <v>2890</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="28">
+        <f>B1*B10+(1-B1)*120</f>
+        <v>204</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:E12" si="0">C1*C10+(1-C1)*120</f>
+        <v>197.7</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>234</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" si="0"/>
+        <v>206.1</v>
+      </c>
+      <c r="F12" s="28">
+        <f>F1*F10+(1-F1)*120</f>
+        <v>232</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" ref="G12:I12" si="1">G1*G10+(1-G1)*120</f>
+        <v>223.6</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>272</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="1"/>
+        <v>234.8</v>
+      </c>
+      <c r="J12" s="28">
+        <f>J1*J10+(1-J1)*120</f>
+        <v>260</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" ref="K12:M12" si="2">K1*K10+(1-K1)*120</f>
+        <v>249.5</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="2"/>
+        <v>310</v>
+      </c>
+      <c r="M12" s="29">
+        <f t="shared" si="2"/>
+        <v>263.5</v>
+      </c>
+      <c r="N12" s="28">
+        <f>N1*N10+(1-N1)*120</f>
+        <v>209.6</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" ref="O12:Q12" si="3">O1*O10+(1-O1)*120</f>
+        <v>202.88</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="3"/>
+        <v>241.6</v>
+      </c>
+      <c r="Q12" s="29">
+        <f t="shared" si="3"/>
+        <v>211.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="28">
+        <f>900*(1-B1)+B11*B1</f>
+        <v>1800</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ref="C13:E13" si="4">900*(1-C1)+C11*C1</f>
+        <v>1044</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="4"/>
+        <v>1230</v>
+      </c>
+      <c r="E13" s="29">
+        <f t="shared" si="4"/>
+        <v>1497</v>
+      </c>
+      <c r="F13" s="28">
+        <f>900*(1-F1)+F11*F1</f>
+        <v>2100</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" ref="G13:I13" si="5">900*(1-G1)+G11*G1</f>
+        <v>1092</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="5"/>
+        <v>1340</v>
+      </c>
+      <c r="I13" s="29">
+        <f t="shared" si="5"/>
+        <v>1696</v>
+      </c>
+      <c r="J13" s="28">
+        <f>900*(1-J1)+J11*J1</f>
+        <v>2400</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" ref="K13:M13" si="6">900*(1-K1)+K11*K1</f>
+        <v>1140</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="6"/>
+        <v>1450</v>
+      </c>
+      <c r="M13" s="29">
+        <f t="shared" si="6"/>
+        <v>1895</v>
+      </c>
+      <c r="N13" s="28">
+        <f>900*(1-N1)+N11*N1</f>
+        <v>1860</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" ref="O13:Q13" si="7">900*(1-O1)+O11*O1</f>
+        <v>1053.5999999999999</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="7"/>
+        <v>1252</v>
+      </c>
+      <c r="Q13" s="29">
+        <f t="shared" si="7"/>
+        <v>1536.8000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="28">
+        <f>B12/B9</f>
+        <v>68</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:E14" si="8">C12/C9</f>
+        <v>50.050632911392398</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="8"/>
+        <v>117</v>
+      </c>
+      <c r="E14" s="29">
+        <f t="shared" si="8"/>
+        <v>10.678756476683937</v>
+      </c>
+      <c r="F14" s="28">
+        <f>F12/F9</f>
+        <v>77.333333333333329</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" ref="G14:I14" si="9">G12/G9</f>
+        <v>56.607594936708857</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="9"/>
+        <v>136</v>
+      </c>
+      <c r="I14" s="29">
+        <f t="shared" si="9"/>
+        <v>12.165803108808291</v>
+      </c>
+      <c r="J14" s="28">
+        <f>J12/J9</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" ref="K14:M14" si="10">K12/K9</f>
+        <v>63.164556962025316</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="10"/>
+        <v>155</v>
+      </c>
+      <c r="M14" s="29">
+        <f t="shared" si="10"/>
+        <v>13.652849740932641</v>
+      </c>
+      <c r="N14" s="28">
+        <f>N12/N9</f>
+        <v>69.86666666666666</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" ref="O14:Q14" si="11">O12/O9</f>
+        <v>51.362025316455693</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="11"/>
+        <v>120.8</v>
+      </c>
+      <c r="Q14" s="29">
+        <f t="shared" si="11"/>
+        <v>10.976165803108808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="28">
+        <f>B13/B9</f>
+        <v>600</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" ref="C15:E15" si="12">C13/C9</f>
+        <v>264.30379746835445</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="12"/>
+        <v>615</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="12"/>
+        <v>77.564766839378237</v>
+      </c>
+      <c r="F15" s="28">
+        <f>F13/F9</f>
+        <v>700</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" ref="G15:I15" si="13">G13/G9</f>
+        <v>276.45569620253161</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="13"/>
+        <v>670</v>
+      </c>
+      <c r="I15" s="29">
+        <f t="shared" si="13"/>
+        <v>87.875647668393782</v>
+      </c>
+      <c r="J15" s="28">
+        <f>J13/J9</f>
+        <v>800</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" ref="K15:M15" si="14">K13/K9</f>
+        <v>288.60759493670884</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="14"/>
+        <v>725</v>
+      </c>
+      <c r="M15" s="29">
+        <f t="shared" si="14"/>
+        <v>98.186528497409327</v>
+      </c>
+      <c r="N15" s="28">
+        <f>N13/N9</f>
+        <v>620</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" ref="O15:Q15" si="15">O13/O9</f>
+        <v>266.73417721518985</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="15"/>
+        <v>626</v>
+      </c>
+      <c r="Q15" s="29">
+        <f t="shared" si="15"/>
+        <v>79.62694300518136</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDECDF0-863A-4B0F-8EEC-005766D5F9F8}">
   <dimension ref="B2:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13016,7 +13699,7 @@
       <c r="B2" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="19">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -13027,7 +13710,7 @@
       <c r="B3" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="19">
         <v>1</v>
       </c>
       <c r="D3" t="s">
@@ -13038,7 +13721,7 @@
       <c r="B4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="19">
         <v>9000</v>
       </c>
       <c r="D4" t="s">
@@ -13049,7 +13732,7 @@
       <c r="B5" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="19">
         <v>30000</v>
       </c>
       <c r="D5" t="s">
@@ -13098,7 +13781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C57C47C-2DB5-41EB-897C-E00A092F2D10}">
   <dimension ref="A3:AC38"/>
   <sheetViews>
@@ -13938,6 +14621,22 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{042DAF65-3C25-4A68-8081-C638AE77C5B6}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!C24:F24</xm:f>
+              <xm:sqref>H24</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{839EA5D5-E16D-4E27-B7C7-B5147372F7B5}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -13954,29 +14653,13 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{042DAF65-3C25-4A68-8081-C638AE77C5B6}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!C24:F24</xm:f>
-              <xm:sqref>H24</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C696E5-2114-48AB-AEEF-857595950602}">
   <dimension ref="B19:N28"/>
   <sheetViews>
@@ -13994,18 +14677,18 @@
   </cols>
   <sheetData>
     <row r="19" spans="2:14">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="G19" s="25" t="s">
+      <c r="C19" s="25"/>
+      <c r="G19" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="K19" s="25" t="s">
+      <c r="H19" s="26"/>
+      <c r="K19" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="25"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="6" t="s">
@@ -14075,10 +14758,10 @@
       </c>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="24"/>
+      <c r="C25" s="25"/>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="6" t="s">

</xml_diff>